<commit_message>
Paper and new paper
Terminé el paper "Can commodity prices forecast exchange rates?" y puse otro nuevo
</commit_message>
<xml_diff>
--- a/Revisión de literatura/literature_review.xlsx
+++ b/Revisión de literatura/literature_review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe Ruiz\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0ECB24-F825-4CF2-A988-1FBFFD1B3F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045A4C10-E445-4BFD-B561-6E7EA61C8FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{0FF652F1-D738-497E-889F-D9943026092A}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="123">
   <si>
     <t>Nombre</t>
   </si>
@@ -420,13 +420,19 @@
   </si>
   <si>
     <t>https://bit.ly/3jfkPGX</t>
+  </si>
+  <si>
+    <t>Can oil prices forecast exchange rates?</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0261560615000479</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -508,20 +514,8 @@
       <name val="Candara"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF00B050"/>
-      <name val="Candara"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="9"/>
-      <name val="Candara"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -553,18 +547,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF8F565"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -708,7 +690,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -752,15 +734,12 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1452,8 +1431,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DFC40022-B6E0-5248-892C-DB7F37657C4A}" name="Variables" displayName="Variables" ref="A1:G24" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <autoFilter ref="A1:G24" xr:uid="{DFC40022-B6E0-5248-892C-DB7F37657C4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DFC40022-B6E0-5248-892C-DB7F37657C4A}" name="Variables" displayName="Variables" ref="A1:G25" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="A1:G25" xr:uid="{DFC40022-B6E0-5248-892C-DB7F37657C4A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{5D274B06-4DAE-144E-90B9-0BA3ED60490F}" name="Variable" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
     <tableColumn id="7" xr3:uid="{312D9853-9B84-40C9-B4A4-EDC49298F048}" name="Date" dataDxfId="23" totalsRowDxfId="22"/>
@@ -1805,10 +1784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B040F3FE-2291-4213-9DA7-4BDF5F8EFDCD}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E9" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2062,7 +2041,7 @@
         <v>78</v>
       </c>
       <c r="E14" s="8"/>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="18" t="s">
         <v>116</v>
       </c>
       <c r="G14" s="10" t="s">
@@ -2117,7 +2096,7 @@
         <v>87</v>
       </c>
       <c r="E17" s="9"/>
-      <c r="F17" s="24" t="s">
+      <c r="F17" s="18" t="s">
         <v>116</v>
       </c>
       <c r="G17" s="10" t="s">
@@ -2189,7 +2168,9 @@
         <v>99</v>
       </c>
       <c r="E21" s="9"/>
-      <c r="F21" s="17"/>
+      <c r="F21" s="18" t="s">
+        <v>116</v>
+      </c>
       <c r="G21" s="10" t="s">
         <v>98</v>
       </c>
@@ -2248,9 +2229,28 @@
         <v>119</v>
       </c>
       <c r="E24" s="14"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="23" t="s">
+      <c r="F24" s="21"/>
+      <c r="G24" s="22" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="13">
+        <v>2015</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E25" s="14"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="23" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2274,12 +2274,13 @@
     <hyperlink ref="G22" r:id="rId17" display="https://pubs.aeaweb.org/doi/pdfplus/10.1257/mac.20150317" xr:uid="{5E64A5A2-269E-4CA1-A444-9870A82D4EC4}"/>
     <hyperlink ref="G23" r:id="rId18" xr:uid="{90A62FB6-09E5-40EA-A000-43224542DA37}"/>
     <hyperlink ref="G24" r:id="rId19" xr:uid="{878BAD48-7820-46C6-BF61-4BD85CA021E5}"/>
+    <hyperlink ref="G25" r:id="rId20" xr:uid="{6FABA652-BAB5-429D-A673-DEBAB0B534CC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
-  <legacyDrawing r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
+  <legacyDrawing r:id="rId22"/>
   <tableParts count="1">
-    <tablePart r:id="rId22"/>
+    <tablePart r:id="rId23"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>